<commit_message>
*Sacados combo charts y comentarios para datos madrid mergeados *Aplicacion qliksense finalizada. Creado un readme con instrucciones para su instalación . Se incluyen extensiones necesarias para ver todos los objetos. Se incluyen pantallazos para describir las funcionalidades de cada dashboard.
</commit_message>
<xml_diff>
--- a/visualizaciones qlik/Otros/AQI_SCALE.xlsx
+++ b/visualizaciones qlik/Otros/AQI_SCALE.xlsx
@@ -5,28 +5,37 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaume\Documents\0.CURSO BIG DATA.MIRADAX TELEFONICA\Proyectos repositorios git\ProyectoBigData\datosContaminacionBarcelona\datosmadrid_aqicn_org\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaume\Documents\0.CURSO BIG DATA.MIRADAX TELEFONICA\Proyectos repositorios git\ProyectoBigData\visualizaciones qlik\Otros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190E97C4-8595-4D61-8863-20B44DA8D7B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AB1D55-8FC1-40BF-B3BB-8F1A19A08CD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="855" yWindow="2475" windowWidth="8970" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="SOURCE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>AQI</t>
   </si>
@@ -125,6 +134,30 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>#009966</t>
+  </si>
+  <si>
+    <t>#ffdd33</t>
+  </si>
+  <si>
+    <t>#ff9933</t>
+  </si>
+  <si>
+    <t>#cc0033</t>
+  </si>
+  <si>
+    <t>#660099</t>
+  </si>
+  <si>
+    <t>#7e0035</t>
   </si>
 </sst>
 </file>
@@ -520,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +564,7 @@
     <col min="1" max="4" width="58.85546875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,8 +592,14 @@
       <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -588,8 +627,15 @@
       <c r="I2">
         <v>102</v>
       </c>
+      <c r="J2" t="str">
+        <f>_xlfn.CONCAT(G2,",",H2,",",I2)</f>
+        <v>0,153,102</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -609,7 +655,7 @@
         <v>100</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="H3">
         <v>222</v>
@@ -617,8 +663,15 @@
       <c r="I3">
         <v>51</v>
       </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J6" si="0">_xlfn.CONCAT(G3,",",H3,",",I3)</f>
+        <v>255,222,51</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -646,8 +699,15 @@
       <c r="I4">
         <v>51</v>
       </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>255,153,51</v>
+      </c>
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -675,8 +735,15 @@
       <c r="I5">
         <v>51</v>
       </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>204,0,51</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -704,8 +771,15 @@
       <c r="I6" s="10">
         <v>153</v>
       </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>102,0,153</v>
+      </c>
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -732,6 +806,13 @@
       </c>
       <c r="I7" s="10">
         <v>53</v>
+      </c>
+      <c r="J7" t="str">
+        <f>_xlfn.CONCAT(G7,",",H7,",",I7)</f>
+        <v>126,0,53</v>
+      </c>
+      <c r="K7" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>